<commit_message>
update name of 贤慕大道
Fix wrong character
</commit_message>
<xml_diff>
--- a/FallowayStations.xlsx
+++ b/FallowayStations.xlsx
@@ -199,7 +199,7 @@
     <t>俊霖路</t>
   </si>
   <si>
-    <t>贤墓大道</t>
+    <t>贤慕大道</t>
   </si>
 </sst>
 </file>
@@ -565,7 +565,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>